<commit_message>
day 14 part 2
</commit_message>
<xml_diff>
--- a/aoc/inputs.xlsx
+++ b/aoc/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafa_\Desktop\advent-of-code-2020\aoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C6C75E-FB21-4B74-8A47-35F4D1F317B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F2C26F-1B8D-4DCC-BE96-BF6AC5FC1AA2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="13" xr2:uid="{A0D34D6D-63E3-4BFB-96C8-C1778D293801}"/>
   </bookViews>
@@ -29,7 +29,6 @@
     <sheet name="Sheet14" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7392" uniqueCount="6072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7396" uniqueCount="6076">
   <si>
     <t>2-4 r: prrmspx</t>
   </si>
@@ -18264,6 +18263,18 @@
   </si>
   <si>
     <t>mem[8] = 0</t>
+  </si>
+  <si>
+    <t>mask = 000000000000000000000000000000X1001X</t>
+  </si>
+  <si>
+    <t>mem[42] = 100</t>
+  </si>
+  <si>
+    <t>mask = 00000000000000000000000000000000X0XX</t>
+  </si>
+  <si>
+    <t>mem[26] = 1</t>
   </si>
 </sst>
 </file>
@@ -25001,23 +25012,26 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03FDF991-65CE-4A8A-8863-96E33FAA9CA1}">
-  <dimension ref="A1:G576"/>
+  <dimension ref="A1:K576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>5492</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6068</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="I1" s="2" t="s">
+        <v>6072</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
         <v>5493</v>
       </c>
@@ -25032,79 +25046,92 @@
         <f>+""""&amp;_xlfn.TEXTJOIN(""", """,FALSE,E1:E4)&amp;""""</f>
         <v>"mask = XXXXXXXXXXXXXXXXXXXXXXXXXXXXX1XXXX0X", "mem[8] = 11", "mem[7] = 101", "mem[8] = 0"</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" s="2" t="s">
+        <v>6073</v>
+      </c>
+      <c r="K2" t="str">
+        <f>+""""&amp;_xlfn.TEXTJOIN(""", """,FALSE,I1:I4)&amp;""""</f>
+        <v>"mask = 000000000000000000000000000000X1001X", "mem[42] = 100", "mask = 00000000000000000000000000000000X0XX", "mem[26] = 1"</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
         <v>5494</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6070</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I3" s="2" t="s">
+        <v>6074</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
         <v>5495</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6071</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="I4" s="2" t="s">
+        <v>6075</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
         <v>5496</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="A6" s="2" t="s">
         <v>5497</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
         <v>5498</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:11">
       <c r="A8" s="2" t="s">
         <v>5499</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:11">
       <c r="A9" s="2" t="s">
         <v>5500</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
         <v>5501</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:11">
       <c r="A11" s="2" t="s">
         <v>5502</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
         <v>5503</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
         <v>5504</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
         <v>5505</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
         <v>5506</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
         <v>5507</v>
       </c>

</xml_diff>